<commit_message>
fin d'implémentation de la webapp, génération du war de la Webapp version 1.0
</commit_message>
<xml_diff>
--- a/ActionsStruts.xlsx
+++ b/ActionsStruts.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$H$12</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
     <t>jsp</t>
   </si>
@@ -416,6 +416,24 @@
   </si>
   <si>
     <t>livre.ProlongerPretAction / actionAjax</t>
+  </si>
+  <si>
+    <t>voirDispo_ajax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voir la dispo d'un livre dans le différente bibliothèque de la ville </t>
+  </si>
+  <si>
+    <t>livre.RechercherAction / actionAjax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(JSON) </t>
+  </si>
+  <si>
+    <t>livre.DispoAction / actionAjax</t>
+  </si>
+  <si>
+    <t>int id</t>
   </si>
 </sst>
 </file>
@@ -910,10 +928,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.5703125" defaultRowHeight="15"/>
@@ -1265,7 +1283,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="60">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -1274,7 +1292,9 @@
       <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="E15" s="9" t="s">
         <v>53</v>
       </c>
@@ -1286,38 +1306,61 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30">
-      <c r="A16" s="5" t="s">
-        <v>63</v>
-      </c>
+    <row r="16" spans="1:8" ht="45">
+      <c r="A16" s="14"/>
       <c r="B16" s="11" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>7</v>
+      <c r="F16" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="30">
+      <c r="A17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H16">
+  <autoFilter ref="A1:H17">
     <filterColumn colId="3"/>
   </autoFilter>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A4:A10"/>
+    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="landscape" verticalDpi="300" r:id="rId1"/>

</xml_diff>